<commit_message>
PPT and Excel Commit
</commit_message>
<xml_diff>
--- a/Functional_Testing_Group2.xlsx
+++ b/Functional_Testing_Group2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23822"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/888331_cognizant_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\888292\Desktop\Group_2_Identify_Courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{666E6D90-4AB0-4747-8B44-29A1CC298FB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13215" windowHeight="4560" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEST SCENARIO" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="DEFECT REPORT" sheetId="5" r:id="rId3"/>
     <sheet name="RTM" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="228">
   <si>
     <t>Module</t>
   </si>
@@ -528,9 +527,6 @@
     <t>7]Valid Number of employees should be selected.</t>
   </si>
   <si>
-    <t>7]Selected Number of rooms are displayed.</t>
-  </si>
-  <si>
     <t>8]Select how many people to train</t>
   </si>
   <si>
@@ -624,18 +620,6 @@
     <t>TS07.5</t>
   </si>
   <si>
-    <t>Providing JobTitle as "Software Engineer"</t>
-  </si>
-  <si>
-    <t>6]Enter the JobTitle as "Software Engineer"</t>
-  </si>
-  <si>
-    <t>6]JobTitle should be displayed as "Software Engineer".</t>
-  </si>
-  <si>
-    <t>6]JobTitle is displayed as "Software Engineer"</t>
-  </si>
-  <si>
     <t>TS07.6</t>
   </si>
   <si>
@@ -706,13 +690,43 @@
   </si>
   <si>
     <t>Course in English Language</t>
+  </si>
+  <si>
+    <t>Providing JobTitle as "Tester"</t>
+  </si>
+  <si>
+    <t>6]Enter the JobTitle as "Tester"</t>
+  </si>
+  <si>
+    <t>6]JobTitle should be displayed as "Tester".</t>
+  </si>
+  <si>
+    <t>6]JobTitle is displayed as "Tester"</t>
+  </si>
+  <si>
+    <t>Providing Valid values in form</t>
+  </si>
+  <si>
+    <t>3]Enter the Work Email (xyz@udemy.com)</t>
+  </si>
+  <si>
+    <t>3]Email should be displayed</t>
+  </si>
+  <si>
+    <t>3]Email is displayed</t>
+  </si>
+  <si>
+    <t>10]Should navigate to success page</t>
+  </si>
+  <si>
+    <t>10]Navigates to success page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1125,14 +1139,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="7" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="4" customWidth="1"/>
@@ -1142,7 +1156,7 @@
     <col min="6" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1159,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -1173,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1187,7 +1201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1198,7 +1212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1209,7 +1223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1220,7 +1234,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1249,18 +1263,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J141"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D18"/>
+    <sheetView tabSelected="1" topLeftCell="D136" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" customWidth="1"/>
     <col min="4" max="4" width="56.5703125" customWidth="1"/>
     <col min="5" max="5" width="55.85546875" customWidth="1"/>
     <col min="6" max="6" width="61.140625" customWidth="1"/>
@@ -1270,7 +1284,7 @@
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
@@ -1302,7 +1316,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1334,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>38</v>
@@ -1346,7 +1360,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="2"/>
@@ -1366,7 +1380,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>48</v>
@@ -1392,7 +1406,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
@@ -1412,7 +1426,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>52</v>
@@ -1438,7 +1452,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
@@ -1458,7 +1472,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>56</v>
@@ -1484,7 +1498,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1504,7 +1518,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>60</v>
@@ -1530,7 +1544,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -1550,7 +1564,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1582,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>65</v>
@@ -1594,7 +1608,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="2"/>
@@ -1616,7 +1630,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="2"/>
@@ -1636,7 +1650,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>78</v>
@@ -1662,7 +1676,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="2"/>
@@ -1684,7 +1698,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="2"/>
@@ -1704,7 +1718,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="2"/>
@@ -1724,7 +1738,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>83</v>
@@ -1750,7 +1764,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="2"/>
@@ -1772,7 +1786,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="2"/>
@@ -1792,7 +1806,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="2"/>
@@ -1812,7 +1826,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="2"/>
@@ -1832,7 +1846,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="2"/>
@@ -1852,7 +1866,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="2"/>
@@ -1872,7 +1886,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>94</v>
@@ -1898,7 +1912,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="2"/>
@@ -1920,7 +1934,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="2"/>
@@ -1940,7 +1954,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="2"/>
@@ -1960,7 +1974,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="2"/>
@@ -1980,7 +1994,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="2"/>
@@ -2000,7 +2014,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="2"/>
@@ -2020,7 +2034,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="2"/>
@@ -2040,7 +2054,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="2"/>
@@ -2060,7 +2074,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>102</v>
@@ -2086,7 +2100,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="2"/>
@@ -2108,7 +2122,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="2"/>
@@ -2128,7 +2142,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="2"/>
@@ -2148,7 +2162,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="2"/>
@@ -2168,7 +2182,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="2"/>
@@ -2188,7 +2202,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="2"/>
@@ -2208,7 +2222,7 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="2"/>
@@ -2228,7 +2242,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="2"/>
@@ -2248,7 +2262,7 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10" ht="17.25" customHeight="1">
+    <row r="46" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="2"/>
@@ -2266,7 +2280,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1">
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2308,7 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="1"/>
@@ -2316,7 +2330,7 @@
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="11"/>
       <c r="C49" s="1"/>
@@ -2336,7 +2350,7 @@
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="11"/>
       <c r="C50" s="1"/>
@@ -2356,7 +2370,7 @@
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="11"/>
       <c r="C51" s="1"/>
@@ -2376,7 +2390,7 @@
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="11"/>
       <c r="C52" s="1"/>
@@ -2396,7 +2410,7 @@
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="11"/>
       <c r="C53" s="1"/>
@@ -2416,7 +2430,7 @@
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>16</v>
       </c>
@@ -2444,7 +2458,7 @@
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
         <v>71</v>
       </c>
@@ -2463,7 +2477,7 @@
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E56" s="2" t="s">
         <v>75</v>
       </c>
@@ -2479,7 +2493,7 @@
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E57" s="2" t="s">
         <v>80</v>
       </c>
@@ -2495,7 +2509,7 @@
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E58" s="2" t="s">
         <v>85</v>
       </c>
@@ -2511,7 +2525,7 @@
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E59" s="2" t="s">
         <v>129</v>
       </c>
@@ -2527,7 +2541,7 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>19</v>
       </c>
@@ -2555,7 +2569,7 @@
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D61" s="9" t="s">
         <v>71</v>
       </c>
@@ -2574,7 +2588,7 @@
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
         <v>75</v>
       </c>
@@ -2590,7 +2604,7 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E63" s="2" t="s">
         <v>80</v>
       </c>
@@ -2606,7 +2620,7 @@
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E64" s="2" t="s">
         <v>85</v>
       </c>
@@ -2622,7 +2636,7 @@
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E65" s="2" t="s">
         <v>88</v>
       </c>
@@ -2638,7 +2652,7 @@
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E66" s="2" t="s">
         <v>91</v>
       </c>
@@ -2654,7 +2668,7 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E67" s="2" t="s">
         <v>96</v>
       </c>
@@ -2670,7 +2684,7 @@
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E68" s="2" t="s">
         <v>99</v>
       </c>
@@ -2686,7 +2700,7 @@
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>133</v>
       </c>
@@ -2702,7 +2716,7 @@
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>22</v>
       </c>
@@ -2730,7 +2744,7 @@
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D71" s="9" t="s">
         <v>71</v>
       </c>
@@ -2749,7 +2763,7 @@
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E72" s="2" t="s">
         <v>75</v>
       </c>
@@ -2765,7 +2779,7 @@
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E73" s="2" t="s">
         <v>80</v>
       </c>
@@ -2781,7 +2795,7 @@
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E74" s="2" t="s">
         <v>85</v>
       </c>
@@ -2797,7 +2811,7 @@
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E75" s="2" t="s">
         <v>88</v>
       </c>
@@ -2813,7 +2827,7 @@
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E76" s="2" t="s">
         <v>91</v>
       </c>
@@ -2829,7 +2843,7 @@
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E77" s="2" t="s">
         <v>96</v>
       </c>
@@ -2845,7 +2859,7 @@
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E78" s="2" t="s">
         <v>99</v>
       </c>
@@ -2861,7 +2875,7 @@
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>133</v>
       </c>
@@ -2877,7 +2891,7 @@
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
         <v>137</v>
       </c>
@@ -2893,7 +2907,7 @@
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>25</v>
       </c>
@@ -2911,7 +2925,7 @@
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
         <v>140</v>
@@ -2937,7 +2951,7 @@
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="2"/>
@@ -2959,7 +2973,7 @@
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="2"/>
@@ -2981,7 +2995,7 @@
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="2"/>
@@ -3001,7 +3015,7 @@
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="2"/>
@@ -3021,7 +3035,7 @@
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="2"/>
@@ -3041,7 +3055,7 @@
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="4"/>
       <c r="C88" s="2"/>
@@ -3053,7 +3067,7 @@
         <v>162</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>44</v>
@@ -3061,19 +3075,19 @@
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="4"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="H89" s="4" t="s">
         <v>44</v>
@@ -3081,19 +3095,19 @@
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="4"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>44</v>
@@ -3101,19 +3115,19 @@
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="H91" s="4" t="s">
         <v>44</v>
@@ -3121,25 +3135,25 @@
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>174</v>
       </c>
       <c r="D92" s="9" t="s">
         <v>67</v>
       </c>
       <c r="E92" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="H92" s="4" t="s">
         <v>44</v>
@@ -3147,7 +3161,7 @@
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="2"/>
@@ -3155,13 +3169,13 @@
         <v>45</v>
       </c>
       <c r="E93" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="H93" s="4" t="s">
         <v>44</v>
@@ -3169,7 +3183,7 @@
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="2"/>
@@ -3191,7 +3205,7 @@
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="2"/>
@@ -3211,7 +3225,7 @@
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="2"/>
@@ -3231,19 +3245,19 @@
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="H97" s="4" t="s">
         <v>44</v>
@@ -3251,7 +3265,7 @@
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="4"/>
       <c r="C98" s="2"/>
@@ -3263,7 +3277,7 @@
         <v>162</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="H98" s="4" t="s">
         <v>44</v>
@@ -3271,19 +3285,19 @@
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="4"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>44</v>
@@ -3291,19 +3305,19 @@
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>44</v>
@@ -3311,19 +3325,19 @@
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="H101" s="4" t="s">
         <v>44</v>
@@ -3331,13 +3345,13 @@
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="D102" s="9" t="s">
         <v>67</v>
@@ -3357,7 +3371,7 @@
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="2"/>
@@ -3379,7 +3393,7 @@
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="2"/>
@@ -3387,13 +3401,13 @@
         <v>148</v>
       </c>
       <c r="E104" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F104" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>188</v>
       </c>
       <c r="H104" s="4" t="s">
         <v>44</v>
@@ -3401,7 +3415,7 @@
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="2"/>
@@ -3421,7 +3435,7 @@
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="2"/>
@@ -3441,7 +3455,7 @@
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="2"/>
@@ -3461,7 +3475,7 @@
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="2"/>
@@ -3473,73 +3487,73 @@
         <v>162</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="H108" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="15" customHeight="1">
+    <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F109" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G109" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="H109" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="G110" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G110" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="H110" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G111" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="H111" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="D112" s="9" t="s">
         <v>67</v>
@@ -3557,7 +3571,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="2"/>
@@ -3577,7 +3591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="2"/>
@@ -3597,25 +3611,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="G115" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G115" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="H115" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
       <c r="C116" s="2"/>
@@ -3633,7 +3647,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="2"/>
@@ -3651,7 +3665,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="2"/>
@@ -3663,73 +3677,73 @@
         <v>162</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="H118" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F119" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G119" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="H119" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="G120" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G120" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="H120" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F121" s="2" t="s">
+      <c r="G121" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G121" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="H121" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="D122" s="9" t="s">
         <v>67</v>
@@ -3747,7 +3761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="2"/>
@@ -3767,7 +3781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="2"/>
@@ -3787,7 +3801,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="4"/>
       <c r="C125" s="2"/>
@@ -3805,7 +3819,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="2"/>
@@ -3823,25 +3837,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="4"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="H127" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="2"/>
@@ -3853,91 +3867,91 @@
         <v>162</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>163</v>
+        <v>200</v>
       </c>
       <c r="H128" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F129" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F129" s="2" t="s">
+      <c r="G129" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G129" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="H129" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F130" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F130" s="2" t="s">
+      <c r="G130" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G130" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="H130" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F131" s="2" t="s">
+      <c r="G131" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G131" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="H131" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D132" s="9" t="s">
         <v>67</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H132" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="2"/>
@@ -3957,7 +3971,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="2"/>
@@ -3965,7 +3979,7 @@
         <v>148</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>150</v>
@@ -3977,7 +3991,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="2"/>
@@ -3995,7 +4009,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="2"/>
@@ -4013,7 +4027,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="2"/>
@@ -4031,7 +4045,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="2"/>
@@ -4043,63 +4057,243 @@
         <v>162</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H138" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F139" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="G139" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G139" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="H139" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F140" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F140" s="2" t="s">
+      <c r="G140" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G140" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="H140" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F141" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="G141" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G141" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="H141" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D142" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H142" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="4"/>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H143" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="4"/>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H144" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="4"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H145" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="4"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H146" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="4"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H147" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="4"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H148" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="4"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H149" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B150" s="4"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H150" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B151" s="4"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F151" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H151" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4110,14 +4304,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B9A519-F263-4C7A-8E5A-5DDFCAD4CE3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
@@ -4126,36 +4320,36 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" customHeight="1">
+    <row r="1" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>209</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>214</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>37</v>
@@ -4163,18 +4357,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="18.5703125" style="2" customWidth="1"/>
@@ -4185,27 +4380,27 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4213,7 +4408,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
@@ -4222,9 +4417,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">

</xml_diff>